<commit_message>
Make inventory.db in z drive
</commit_message>
<xml_diff>
--- a/Products.xlsx
+++ b/Products.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -472,188 +472,60 @@
           <t>Vendor</t>
         </is>
       </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>PO</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Samsung Galaxy S24</t>
+          <t>1</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>SGS24</t>
+          <t>1</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>1199</v>
+        <v>1</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>pcs</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Flagship Samsung phone</t>
+          <t>1</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>A2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="G2" t="n">
         <v>1</v>
       </c>
       <c r="H2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>V-SGS24</t>
+          <t>1</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>Samsung</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Logitech Mouse</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>LM01</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>25</v>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>pcs</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Wireless mouse</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>B1</t>
-        </is>
-      </c>
-      <c r="G3" t="n">
-        <v>0</v>
-      </c>
-      <c r="H3" t="n">
-        <v>0</v>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>V-LM01</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>Logitech</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Mechanical Keyboard</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>MK01</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>75</v>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>pcs</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>RGB mechanical keyboard</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>B2</t>
-        </is>
-      </c>
-      <c r="G4" t="n">
-        <v>0</v>
-      </c>
-      <c r="H4" t="n">
-        <v>0</v>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>V-MK01</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>Corsair</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>HDMI Cable</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>HC01</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>10</v>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>pcs</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>High-speed HDMI cable</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>C1</t>
-        </is>
-      </c>
-      <c r="G5" t="n">
-        <v>1</v>
-      </c>
-      <c r="H5" t="n">
-        <v>0</v>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>V-HC01</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>Belkin</t>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
     </row>

</xml_diff>